<commit_message>
Syntax changes to sector
</commit_message>
<xml_diff>
--- a/frontend/static/Fundamental_Info.xlsx
+++ b/frontend/static/Fundamental_Info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesse\Desktop\Financial-Advisor-Senior-Project\frontend\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A60D3D0-5442-40FD-9AB2-97B63AEDB3D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD3086E-7B35-4C95-9D04-671482643471}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -387,7 +387,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>